<commit_message>
Sending batch email Dynamic Timestamps
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>lmonica1112@gmail.com</t>
+  </si>
+  <si>
+    <t>lumimonika2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1617,7 +1620,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>8</v>

</xml_diff>